<commit_message>
small changes to prototype
</commit_message>
<xml_diff>
--- a/work products/dsl_prototype.xlsx
+++ b/work products/dsl_prototype.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Mainframe" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -530,7 +531,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -591,7 +592,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1">
-        <f>SUM(B3:F3)</f>
+        <f t="shared" ref="H3:H10" si="0">SUM(B3:F3)</f>
         <v>2</v>
       </c>
     </row>
@@ -608,7 +609,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
-        <f>SUM(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -625,7 +626,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1">
-        <f>SUM(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -640,7 +641,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1">
-        <f>SUM(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -655,7 +656,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1">
-        <f>SUM(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -670,7 +671,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1">
-        <f>SUM(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -685,7 +686,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1">
-        <f>SUM(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -702,7 +703,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1">
-        <f>SUM(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -843,4 +844,28 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <f>Mainframe!C11</f>
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with work from meeting
</commit_message>
<xml_diff>
--- a/work products/dsl_prototype.xlsx
+++ b/work products/dsl_prototype.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,14 +650,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -717,7 +719,7 @@
       </c>
       <c r="C11" s="1">
         <f>SUM(C3:C10)*C2</f>
-        <v>1.5</v>
+        <v>10.5</v>
       </c>
       <c r="D11" s="1">
         <f>SUM(D3:D10)*D2</f>
@@ -736,7 +738,7 @@
       </c>
       <c r="H11" s="1">
         <f>SUM(H3:H10)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -753,7 +755,7 @@
       </c>
       <c r="H14">
         <f>SUM(B11:F11) +H13</f>
-        <v>18.5</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -817,7 +819,7 @@
       </c>
       <c r="E22">
         <f>IF(B11+C11&lt;8,0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="4:5" ht="45">
@@ -831,7 +833,7 @@
       </c>
       <c r="E25" t="str">
         <f>IF(SUM(E17:E22) = 0, "Consistent", "Not Consistent")</f>
-        <v>Consistent</v>
+        <v>Not Consistent</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +859,7 @@
     <row r="1" spans="1:1">
       <c r="A1">
         <f>Mainframe!C11</f>
-        <v>1.5</v>
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>